<commit_message>
despesas com pessoal updted
</commit_message>
<xml_diff>
--- a/auxiliar/dtp_empenhos_terceirizacao.xlsx
+++ b/auxiliar/dtp_empenhos_terceirizacao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everton\Desktop\Sistemas\rptgen\auxiliar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12776409-D2D6-4D55-8283-A301FD7C4F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153629C7-C1A4-4E92-A9B0-AE9CA4ECE8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A1238923-C8BC-4787-9A83-0D45384E9B95}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E3D808-D402-4945-BD96-5457776190CA}" name="EmpenhosTerceirizacao" displayName="EmpenhosTerceirizacao" ref="A1:B14" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B14" xr:uid="{10E3D808-D402-4945-BD96-5457776190CA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{10E3D808-D402-4945-BD96-5457776190CA}" name="EmpenhosTerceirizacao" displayName="EmpenhosTerceirizacao" ref="A1:B23" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B23" xr:uid="{10E3D808-D402-4945-BD96-5457776190CA}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C00875EE-8C7D-43B6-AD73-197A00E396CC}" name="Empenho"/>
     <tableColumn id="2" xr3:uid="{ECD7154E-88CB-428E-BC8E-447C498FF9C1}" name="Ano Empenho"/>
@@ -756,10 +756,10 @@
   <sheetPr>
     <tabColor rgb="FF548135"/>
   </sheetPr>
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B14"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +895,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B13">
         <v>2024</v>
@@ -903,9 +903,81 @@
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>45</v>
+      </c>
+      <c r="B14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>1499</v>
       </c>
-      <c r="B14">
+      <c r="B15">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3008</v>
+      </c>
+      <c r="B16">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4005</v>
+      </c>
+      <c r="B17">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4021</v>
+      </c>
+      <c r="B18">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>6926</v>
+      </c>
+      <c r="B19">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7108</v>
+      </c>
+      <c r="B20">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7109</v>
+      </c>
+      <c r="B21">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>8657</v>
+      </c>
+      <c r="B22">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8684</v>
+      </c>
+      <c r="B23">
         <v>2024</v>
       </c>
     </row>

</xml_diff>